<commit_message>
SU maj raideur ARB
</commit_message>
<xml_diff>
--- a/SU_Suspension/08_raideurBAR/ARBdisplacement.xlsx
+++ b/SU_Suspension/08_raideurBAR/ARBdisplacement.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FSAE_invictus\STUF-2020\SU_Suspension\00_configurations points LAS\Invictus_3421\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FSAE_invictus\Ressources2020\SU_Suspension\08_raideurBAR\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -48,9 +48,6 @@
     <t>rocker axis</t>
   </si>
   <si>
-    <t>Invictus3421_v25</t>
-  </si>
-  <si>
     <t>y</t>
   </si>
   <si>
@@ -61,6 +58,9 @@
   </si>
   <si>
     <t>AB</t>
+  </si>
+  <si>
+    <t>Invictus3421_v26</t>
   </si>
 </sst>
 </file>
@@ -181,14 +181,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -197,15 +215,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Migliaia" xfId="1" builtinId="3"/>
@@ -479,37 +488,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>-15.680000000000007</c:v>
+                  <c:v>-15.180000000000007</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-12.620000000000005</c:v>
+                  <c:v>-12.099999999999994</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-9.5399999999999636</c:v>
+                  <c:v>-9.0600000000000307</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-6.3999999999999773</c:v>
+                  <c:v>-6.0200000000000102</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-3.2400000000000091</c:v>
+                  <c:v>-3.0100000000000193</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.2799999999999727</c:v>
+                  <c:v>3.0100000000000193</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6.6400000000000432</c:v>
+                  <c:v>6.0200000000000102</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>10.079999999999984</c:v>
+                  <c:v>9.0600000000000307</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>13.620000000000005</c:v>
+                  <c:v>12.099999999999994</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>17.259999999999991</c:v>
+                  <c:v>15.180000000000007</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -660,37 +669,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>-16.100000000000023</c:v>
+                  <c:v>-17</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-13.019999999999982</c:v>
+                  <c:v>-13.599999999999966</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-9.8600000000000136</c:v>
+                  <c:v>-10.190000000000055</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-6.6599999999999682</c:v>
+                  <c:v>-6.7999999999999545</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-3.3600000000000136</c:v>
+                  <c:v>-3.3899999999999864</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.4199999999999591</c:v>
+                  <c:v>3.3899999999999864</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6.9399999999999409</c:v>
+                  <c:v>6.7999999999999545</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>10.520000000000095</c:v>
+                  <c:v>10.190000000000055</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>14.17999999999995</c:v>
+                  <c:v>13.599999999999966</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>17.899999999999977</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -705,11 +714,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-431399392"/>
-        <c:axId val="-431398848"/>
+        <c:axId val="-213523552"/>
+        <c:axId val="-213522464"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-431399392"/>
+        <c:axId val="-213523552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -752,12 +761,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-431398848"/>
+        <c:crossAx val="-213522464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-431398848"/>
+        <c:axId val="-213522464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -800,7 +809,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-431399392"/>
+        <c:crossAx val="-213523552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1815,10 +1824,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J27"/>
+  <dimension ref="A1:R30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:K1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T24" sqref="T24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1828,26 +1837,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6" t="s">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="6"/>
-      <c r="E1" s="7" t="s">
+      <c r="D1" s="10"/>
+      <c r="E1" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="14"/>
+      <c r="G1" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="12"/>
+      <c r="I1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="8"/>
-      <c r="G1" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="10"/>
-      <c r="I1" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="12"/>
+      <c r="J1" s="7"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1857,22 +1866,22 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="E2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="G2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="I2" s="2"/>
       <c r="J2" s="2" t="s">
@@ -1887,28 +1896,32 @@
         <v>2.5</v>
       </c>
       <c r="C3">
-        <v>242.07</v>
+        <v>227.27</v>
       </c>
       <c r="D3">
-        <v>161.06</v>
+        <v>160.77000000000001</v>
       </c>
       <c r="E3" s="5">
-        <f>C3-G3</f>
-        <v>39.22999999999999</v>
+        <f t="shared" ref="E3:E13" si="0">C3-G3</f>
+        <v>44.41</v>
       </c>
       <c r="F3" s="5">
-        <f>D3-H3</f>
-        <v>-7.8400000000000034</v>
+        <f t="shared" ref="F3:F13" si="1">D3-H3</f>
+        <v>-7.25</v>
       </c>
       <c r="G3">
-        <v>202.84</v>
+        <v>182.86</v>
       </c>
       <c r="H3">
-        <v>168.9</v>
+        <v>168.02</v>
+      </c>
+      <c r="I3" s="5">
+        <f t="shared" ref="I3:I7" si="2">F3</f>
+        <v>-7.25</v>
       </c>
       <c r="J3">
-        <f>F3*2</f>
-        <v>-15.680000000000007</v>
+        <f>I3-I13</f>
+        <v>-15.180000000000007</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -1919,28 +1932,32 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <v>242.81</v>
+        <v>227.94</v>
       </c>
       <c r="D4">
-        <v>160.82</v>
+        <v>160.59</v>
       </c>
       <c r="E4" s="5">
-        <f>C4-G4</f>
-        <v>39.5</v>
+        <f t="shared" si="0"/>
+        <v>44.620000000000005</v>
       </c>
       <c r="F4" s="5">
-        <f>D4-H4</f>
-        <v>-6.3100000000000023</v>
+        <f t="shared" si="1"/>
+        <v>-5.8400000000000034</v>
       </c>
       <c r="G4">
-        <v>203.31</v>
+        <v>183.32</v>
       </c>
       <c r="H4">
-        <v>167.13</v>
+        <v>166.43</v>
+      </c>
+      <c r="I4" s="5">
+        <f t="shared" si="2"/>
+        <v>-5.8400000000000034</v>
       </c>
       <c r="J4">
-        <f t="shared" ref="J4:J13" si="0">F4*2</f>
-        <v>-12.620000000000005</v>
+        <f>I4-I12</f>
+        <v>-12.099999999999994</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1951,28 +1968,32 @@
         <v>1.5</v>
       </c>
       <c r="C5">
-        <v>243.47</v>
+        <v>228.54</v>
       </c>
       <c r="D5">
-        <v>160.58000000000001</v>
+        <v>160.41999999999999</v>
       </c>
       <c r="E5" s="5">
-        <f>C5-G5</f>
-        <v>39.72</v>
+        <f t="shared" si="0"/>
+        <v>44.78</v>
       </c>
       <c r="F5" s="5">
-        <f>D5-H5</f>
-        <v>-4.7699999999999818</v>
+        <f t="shared" si="1"/>
+        <v>-4.410000000000025</v>
       </c>
       <c r="G5">
-        <v>203.75</v>
+        <v>183.76</v>
       </c>
       <c r="H5">
-        <v>165.35</v>
+        <v>164.83</v>
+      </c>
+      <c r="I5" s="5">
+        <f t="shared" si="2"/>
+        <v>-4.410000000000025</v>
       </c>
       <c r="J5">
-        <f t="shared" si="0"/>
-        <v>-9.5399999999999636</v>
+        <f>I5-I11</f>
+        <v>-9.0600000000000307</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -1983,28 +2004,32 @@
         <v>1</v>
       </c>
       <c r="C6">
-        <v>244.06</v>
+        <v>229.09</v>
       </c>
       <c r="D6">
-        <v>160.37</v>
+        <v>160.26</v>
       </c>
       <c r="E6" s="5">
-        <f>C6-G6</f>
-        <v>39.879999999999995</v>
+        <f t="shared" si="0"/>
+        <v>44.900000000000006</v>
       </c>
       <c r="F6" s="5">
-        <f>D6-H6</f>
-        <v>-3.1999999999999886</v>
+        <f t="shared" si="1"/>
+        <v>-2.960000000000008</v>
       </c>
       <c r="G6">
-        <v>204.18</v>
+        <v>184.19</v>
       </c>
       <c r="H6">
-        <v>163.57</v>
+        <v>163.22</v>
+      </c>
+      <c r="I6" s="5">
+        <f t="shared" si="2"/>
+        <v>-2.960000000000008</v>
       </c>
       <c r="J6">
-        <f t="shared" si="0"/>
-        <v>-6.3999999999999773</v>
+        <f>I6-I10</f>
+        <v>-6.0200000000000102</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -2015,28 +2040,32 @@
         <v>0.5</v>
       </c>
       <c r="C7">
-        <v>244.57</v>
+        <v>229.58</v>
       </c>
       <c r="D7">
-        <v>160.16999999999999</v>
+        <v>160.12</v>
       </c>
       <c r="E7" s="5">
-        <f>C7-G7</f>
-        <v>39.97</v>
+        <f t="shared" si="0"/>
+        <v>44.980000000000018</v>
       </c>
       <c r="F7" s="5">
-        <f>D7-H7</f>
-        <v>-1.6200000000000045</v>
+        <f t="shared" si="1"/>
+        <v>-1.4900000000000091</v>
       </c>
       <c r="G7">
-        <v>204.6</v>
+        <v>184.6</v>
       </c>
       <c r="H7">
-        <v>161.79</v>
+        <v>161.61000000000001</v>
+      </c>
+      <c r="I7" s="5">
+        <f t="shared" si="2"/>
+        <v>-1.4900000000000091</v>
       </c>
       <c r="J7">
-        <f t="shared" si="0"/>
-        <v>-3.2400000000000091</v>
+        <f>I7-I9</f>
+        <v>-3.0100000000000193</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -2046,28 +2075,32 @@
       <c r="B8">
         <v>0</v>
       </c>
-      <c r="C8" s="3">
-        <v>245</v>
-      </c>
-      <c r="D8" s="3">
+      <c r="C8">
+        <v>230</v>
+      </c>
+      <c r="D8">
         <v>160</v>
       </c>
       <c r="E8" s="5">
-        <f>C8-G8</f>
-        <v>40</v>
+        <f t="shared" si="0"/>
+        <v>45</v>
       </c>
       <c r="F8" s="5">
-        <f>D8-H8</f>
-        <v>0</v>
-      </c>
-      <c r="G8" s="3">
-        <v>205</v>
-      </c>
-      <c r="H8" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>185</v>
+      </c>
+      <c r="H8">
         <v>160</v>
       </c>
+      <c r="I8" s="5">
+        <f>F8</f>
+        <v>0</v>
+      </c>
       <c r="J8">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="J8" si="3">F8*2</f>
         <v>0</v>
       </c>
     </row>
@@ -2079,28 +2112,32 @@
         <v>-0.5</v>
       </c>
       <c r="C9">
-        <v>245.35</v>
+        <v>230.36</v>
       </c>
       <c r="D9">
-        <v>159.85</v>
+        <v>159.9</v>
       </c>
       <c r="E9" s="5">
-        <f>C9-G9</f>
-        <v>39.97</v>
+        <f t="shared" si="0"/>
+        <v>44.970000000000027</v>
       </c>
       <c r="F9" s="5">
-        <f>D9-H9</f>
-        <v>1.6399999999999864</v>
+        <f t="shared" si="1"/>
+        <v>1.5200000000000102</v>
       </c>
       <c r="G9">
-        <v>205.38</v>
+        <v>185.39</v>
       </c>
       <c r="H9">
-        <v>158.21</v>
+        <v>158.38</v>
+      </c>
+      <c r="I9" s="5">
+        <f t="shared" ref="I9:I13" si="4">F9</f>
+        <v>1.5200000000000102</v>
       </c>
       <c r="J9">
-        <f t="shared" si="0"/>
-        <v>3.2799999999999727</v>
+        <f>I9-I7</f>
+        <v>3.0100000000000193</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -2111,28 +2148,32 @@
         <v>-1</v>
       </c>
       <c r="C10">
-        <v>245.61</v>
+        <v>230.65</v>
       </c>
       <c r="D10">
-        <v>159.74</v>
+        <v>159.83000000000001</v>
       </c>
       <c r="E10" s="5">
-        <f>C10-G10</f>
-        <v>39.860000000000014</v>
+        <f t="shared" si="0"/>
+        <v>44.890000000000015</v>
       </c>
       <c r="F10" s="5">
-        <f>D10-H10</f>
-        <v>3.3200000000000216</v>
+        <f t="shared" si="1"/>
+        <v>3.0600000000000023</v>
       </c>
       <c r="G10">
-        <v>205.75</v>
+        <v>185.76</v>
       </c>
       <c r="H10">
-        <v>156.41999999999999</v>
+        <v>156.77000000000001</v>
+      </c>
+      <c r="I10" s="5">
+        <f t="shared" si="4"/>
+        <v>3.0600000000000023</v>
       </c>
       <c r="J10">
-        <f t="shared" si="0"/>
-        <v>6.6400000000000432</v>
+        <f>I10-I6</f>
+        <v>6.0200000000000102</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -2143,28 +2184,32 @@
         <v>-1.5</v>
       </c>
       <c r="C11">
-        <v>245.79</v>
+        <v>230.87</v>
       </c>
       <c r="D11">
-        <v>159.66</v>
+        <v>159.79</v>
       </c>
       <c r="E11" s="5">
-        <f>C11-G11</f>
-        <v>39.679999999999978</v>
+        <f t="shared" si="0"/>
+        <v>44.759999999999991</v>
       </c>
       <c r="F11" s="5">
-        <f>D11-H11</f>
-        <v>5.039999999999992</v>
+        <f t="shared" si="1"/>
+        <v>4.6500000000000057</v>
       </c>
       <c r="G11">
-        <v>206.11</v>
+        <v>186.11</v>
       </c>
       <c r="H11">
-        <v>154.62</v>
+        <v>155.13999999999999</v>
+      </c>
+      <c r="I11" s="5">
+        <f t="shared" si="4"/>
+        <v>4.6500000000000057</v>
       </c>
       <c r="J11">
-        <f t="shared" si="0"/>
-        <v>10.079999999999984</v>
+        <f>I11-I5</f>
+        <v>9.0600000000000307</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -2175,28 +2220,32 @@
         <v>-2</v>
       </c>
       <c r="C12">
-        <v>245.86</v>
+        <v>231.02</v>
       </c>
       <c r="D12">
-        <v>159.63</v>
+        <v>159.78</v>
       </c>
       <c r="E12" s="5">
-        <f>C12-G12</f>
-        <v>39.420000000000016</v>
+        <f t="shared" si="0"/>
+        <v>44.56</v>
       </c>
       <c r="F12" s="5">
-        <f>D12-H12</f>
-        <v>6.8100000000000023</v>
+        <f t="shared" si="1"/>
+        <v>6.2599999999999909</v>
       </c>
       <c r="G12">
-        <v>206.44</v>
+        <v>186.46</v>
       </c>
       <c r="H12">
-        <v>152.82</v>
+        <v>153.52000000000001</v>
+      </c>
+      <c r="I12" s="5">
+        <f t="shared" si="4"/>
+        <v>6.2599999999999909</v>
       </c>
       <c r="J12">
-        <f t="shared" si="0"/>
-        <v>13.620000000000005</v>
+        <f>I12-I4</f>
+        <v>12.099999999999994</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -2207,52 +2256,56 @@
         <v>-2.5</v>
       </c>
       <c r="C13">
-        <v>245.82</v>
+        <v>231.08</v>
       </c>
       <c r="D13">
-        <v>159.65</v>
+        <v>159.82</v>
       </c>
       <c r="E13" s="5">
-        <f>C13-G13</f>
-        <v>39.049999999999983</v>
+        <f t="shared" si="0"/>
+        <v>44.300000000000011</v>
       </c>
       <c r="F13" s="5">
-        <f>D13-H13</f>
-        <v>8.6299999999999955</v>
+        <f t="shared" si="1"/>
+        <v>7.9300000000000068</v>
       </c>
       <c r="G13">
-        <v>206.77</v>
+        <v>186.78</v>
       </c>
       <c r="H13">
-        <v>151.02000000000001</v>
+        <v>151.88999999999999</v>
+      </c>
+      <c r="I13" s="5">
+        <f t="shared" si="4"/>
+        <v>7.9300000000000068</v>
       </c>
       <c r="J13">
-        <f t="shared" si="0"/>
-        <v>17.259999999999991</v>
+        <f>I13-I3</f>
+        <v>15.180000000000007</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="10"/>
+      <c r="E15" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" s="6"/>
-      <c r="E15" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F15" s="8"/>
-      <c r="G15" s="9" t="s">
+      <c r="F15" s="14"/>
+      <c r="G15" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H15" s="10"/>
-      <c r="I15" s="13" t="str">
+      <c r="H15" s="12"/>
+      <c r="I15" s="8" t="str">
         <f>I1</f>
-        <v>Invictus3421_v25</v>
-      </c>
-      <c r="J15" s="13"/>
+        <v>Invictus3421_v26</v>
+      </c>
+      <c r="J15" s="9"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -2262,29 +2315,29 @@
         <v>1</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="E16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F16" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="G16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H16" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="I16" s="2"/>
       <c r="J16" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>0</v>
       </c>
@@ -2298,11 +2351,11 @@
         <v>452.82</v>
       </c>
       <c r="E17" s="5">
-        <f>C17-G17</f>
+        <f t="shared" ref="E17:E27" si="5">C17-G17</f>
         <v>28.900000000000006</v>
       </c>
       <c r="F17" s="5">
-        <f>D17-H17</f>
+        <f t="shared" ref="F17:F27" si="6">D17-H17</f>
         <v>-8.0500000000000114</v>
       </c>
       <c r="G17">
@@ -2311,12 +2364,16 @@
       <c r="H17">
         <v>460.87</v>
       </c>
+      <c r="I17" s="5">
+        <f t="shared" ref="I17:I27" si="7">F17</f>
+        <v>-8.0500000000000114</v>
+      </c>
       <c r="J17">
-        <f>F17*2</f>
-        <v>-16.100000000000023</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+        <f>I17-I27</f>
+        <v>-17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>0</v>
       </c>
@@ -2330,11 +2387,11 @@
         <v>452.63</v>
       </c>
       <c r="E18" s="5">
-        <f>C18-G18</f>
+        <f t="shared" si="5"/>
         <v>29.28</v>
       </c>
       <c r="F18" s="5">
-        <f>D18-H18</f>
+        <f t="shared" si="6"/>
         <v>-6.5099999999999909</v>
       </c>
       <c r="G18">
@@ -2343,12 +2400,16 @@
       <c r="H18">
         <v>459.14</v>
       </c>
+      <c r="I18" s="5">
+        <f t="shared" si="7"/>
+        <v>-6.5099999999999909</v>
+      </c>
       <c r="J18">
-        <f t="shared" ref="J18:J27" si="1">F18*2</f>
-        <v>-13.019999999999982</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+        <f>I18-I26</f>
+        <v>-13.599999999999966</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>0</v>
       </c>
@@ -2362,11 +2423,11 @@
         <v>452.46</v>
       </c>
       <c r="E19" s="5">
-        <f>C19-G19</f>
+        <f t="shared" si="5"/>
         <v>29.589999999999975</v>
       </c>
       <c r="F19" s="5">
-        <f>D19-H19</f>
+        <f t="shared" si="6"/>
         <v>-4.9300000000000068</v>
       </c>
       <c r="G19">
@@ -2375,12 +2436,16 @@
       <c r="H19">
         <v>457.39</v>
       </c>
+      <c r="I19" s="5">
+        <f t="shared" si="7"/>
+        <v>-4.9300000000000068</v>
+      </c>
       <c r="J19">
-        <f t="shared" si="1"/>
-        <v>-9.8600000000000136</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+        <f>I19-I25</f>
+        <v>-10.190000000000055</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>0</v>
       </c>
@@ -2394,11 +2459,11 @@
         <v>452.29</v>
       </c>
       <c r="E20" s="5">
-        <f>C20-G20</f>
+        <f t="shared" si="5"/>
         <v>29.810000000000002</v>
       </c>
       <c r="F20" s="5">
-        <f>D20-H20</f>
+        <f t="shared" si="6"/>
         <v>-3.3299999999999841</v>
       </c>
       <c r="G20">
@@ -2407,12 +2472,34 @@
       <c r="H20">
         <v>455.62</v>
       </c>
+      <c r="I20" s="5">
+        <f t="shared" si="7"/>
+        <v>-3.3299999999999841</v>
+      </c>
       <c r="J20">
-        <f t="shared" si="1"/>
-        <v>-6.6599999999999682</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+        <f>I20-I24</f>
+        <v>-6.7999999999999545</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <v>2.5</v>
+      </c>
+      <c r="O20">
+        <v>0</v>
+      </c>
+      <c r="P20">
+        <v>-7.2733999999999996</v>
+      </c>
+      <c r="Q20">
+        <v>227.27</v>
+      </c>
+      <c r="R20">
+        <v>160.77000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>0</v>
       </c>
@@ -2426,11 +2513,11 @@
         <v>452.14</v>
       </c>
       <c r="E21" s="5">
-        <f>C21-G21</f>
+        <f t="shared" si="5"/>
         <v>29.950000000000017</v>
       </c>
       <c r="F21" s="5">
-        <f>D21-H21</f>
+        <f t="shared" si="6"/>
         <v>-1.6800000000000068</v>
       </c>
       <c r="G21">
@@ -2439,12 +2526,34 @@
       <c r="H21">
         <v>453.82</v>
       </c>
+      <c r="I21" s="5">
+        <f t="shared" si="7"/>
+        <v>-1.6800000000000068</v>
+      </c>
       <c r="J21">
-        <f t="shared" si="1"/>
-        <v>-3.3600000000000136</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+        <f>I21-I23</f>
+        <v>-3.3899999999999864</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <v>2</v>
+      </c>
+      <c r="O21">
+        <v>0</v>
+      </c>
+      <c r="P21">
+        <v>-7.2271000000000001</v>
+      </c>
+      <c r="Q21">
+        <v>227.94</v>
+      </c>
+      <c r="R21">
+        <v>160.59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>0</v>
       </c>
@@ -2458,11 +2567,11 @@
         <v>452</v>
       </c>
       <c r="E22" s="5">
-        <f>C22-G22</f>
+        <f t="shared" si="5"/>
         <v>30</v>
       </c>
       <c r="F22" s="5">
-        <f>D22-H22</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="G22" s="3">
@@ -2471,12 +2580,34 @@
       <c r="H22" s="4">
         <v>452</v>
       </c>
+      <c r="I22" s="5">
+        <f>F22</f>
+        <v>0</v>
+      </c>
       <c r="J22">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" ref="J22" si="8">F22*2</f>
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
+      </c>
+      <c r="N22">
+        <v>1.5</v>
+      </c>
+      <c r="O22">
+        <v>0</v>
+      </c>
+      <c r="P22">
+        <v>-7.1806000000000001</v>
+      </c>
+      <c r="Q22">
+        <v>228.54</v>
+      </c>
+      <c r="R22">
+        <v>160.41999999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>0</v>
       </c>
@@ -2490,11 +2621,11 @@
         <v>451.87</v>
       </c>
       <c r="E23" s="5">
-        <f>C23-G23</f>
+        <f t="shared" si="5"/>
         <v>29.949999999999989</v>
       </c>
       <c r="F23" s="5">
-        <f>D23-H23</f>
+        <f t="shared" si="6"/>
         <v>1.7099999999999795</v>
       </c>
       <c r="G23">
@@ -2503,12 +2634,34 @@
       <c r="H23">
         <v>450.16</v>
       </c>
+      <c r="I23" s="5">
+        <f t="shared" si="7"/>
+        <v>1.7099999999999795</v>
+      </c>
       <c r="J23">
-        <f t="shared" si="1"/>
-        <v>3.4199999999999591</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+        <f>I23-I21</f>
+        <v>3.3899999999999864</v>
+      </c>
+      <c r="M23">
+        <v>0</v>
+      </c>
+      <c r="N23">
+        <v>1</v>
+      </c>
+      <c r="O23">
+        <v>0</v>
+      </c>
+      <c r="P23">
+        <v>-7.1338999999999997</v>
+      </c>
+      <c r="Q23">
+        <v>229.09</v>
+      </c>
+      <c r="R23">
+        <v>160.26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>0</v>
       </c>
@@ -2522,11 +2675,11 @@
         <v>451.76</v>
       </c>
       <c r="E24" s="5">
-        <f>C24-G24</f>
+        <f t="shared" si="5"/>
         <v>29.800000000000011</v>
       </c>
       <c r="F24" s="5">
-        <f>D24-H24</f>
+        <f t="shared" si="6"/>
         <v>3.4699999999999704</v>
       </c>
       <c r="G24">
@@ -2535,12 +2688,34 @@
       <c r="H24">
         <v>448.29</v>
       </c>
+      <c r="I24" s="5">
+        <f t="shared" si="7"/>
+        <v>3.4699999999999704</v>
+      </c>
       <c r="J24">
-        <f t="shared" si="1"/>
-        <v>6.9399999999999409</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+        <f>I24-I20</f>
+        <v>6.7999999999999545</v>
+      </c>
+      <c r="M24">
+        <v>0</v>
+      </c>
+      <c r="N24">
+        <v>0.5</v>
+      </c>
+      <c r="O24">
+        <v>0</v>
+      </c>
+      <c r="P24">
+        <v>-7.0869999999999997</v>
+      </c>
+      <c r="Q24">
+        <v>229.58</v>
+      </c>
+      <c r="R24">
+        <v>160.12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>0</v>
       </c>
@@ -2554,11 +2729,11 @@
         <v>451.66</v>
       </c>
       <c r="E25" s="5">
-        <f>C25-G25</f>
+        <f t="shared" si="5"/>
         <v>29.53</v>
       </c>
       <c r="F25" s="5">
-        <f>D25-H25</f>
+        <f t="shared" si="6"/>
         <v>5.2600000000000477</v>
       </c>
       <c r="G25">
@@ -2567,12 +2742,34 @@
       <c r="H25">
         <v>446.4</v>
       </c>
+      <c r="I25" s="5">
+        <f t="shared" si="7"/>
+        <v>5.2600000000000477</v>
+      </c>
       <c r="J25">
-        <f t="shared" si="1"/>
-        <v>10.520000000000095</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+        <f>I25-I19</f>
+        <v>10.190000000000055</v>
+      </c>
+      <c r="M25">
+        <v>0</v>
+      </c>
+      <c r="N25">
+        <v>0</v>
+      </c>
+      <c r="O25">
+        <v>0</v>
+      </c>
+      <c r="P25">
+        <v>-7.04</v>
+      </c>
+      <c r="Q25">
+        <v>230</v>
+      </c>
+      <c r="R25">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>0</v>
       </c>
@@ -2586,11 +2783,11 @@
         <v>451.58</v>
       </c>
       <c r="E26" s="5">
-        <f>C26-G26</f>
+        <f t="shared" si="5"/>
         <v>29.159999999999997</v>
       </c>
       <c r="F26" s="5">
-        <f>D26-H26</f>
+        <f t="shared" si="6"/>
         <v>7.089999999999975</v>
       </c>
       <c r="G26">
@@ -2599,12 +2796,34 @@
       <c r="H26">
         <v>444.49</v>
       </c>
+      <c r="I26" s="5">
+        <f t="shared" si="7"/>
+        <v>7.089999999999975</v>
+      </c>
       <c r="J26">
-        <f t="shared" si="1"/>
-        <v>14.17999999999995</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+        <f>I26-I18</f>
+        <v>13.599999999999966</v>
+      </c>
+      <c r="M26">
+        <v>0</v>
+      </c>
+      <c r="N26">
+        <v>-0.5</v>
+      </c>
+      <c r="O26">
+        <v>0</v>
+      </c>
+      <c r="P26">
+        <v>-6.9928999999999997</v>
+      </c>
+      <c r="Q26">
+        <v>230.36</v>
+      </c>
+      <c r="R26">
+        <v>159.9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>0</v>
       </c>
@@ -2618,11 +2837,11 @@
         <v>451.51</v>
       </c>
       <c r="E27" s="5">
-        <f>C27-G27</f>
+        <f t="shared" si="5"/>
         <v>28.629999999999995</v>
       </c>
       <c r="F27" s="5">
-        <f>D27-H27</f>
+        <f t="shared" si="6"/>
         <v>8.9499999999999886</v>
       </c>
       <c r="G27">
@@ -2631,13 +2850,100 @@
       <c r="H27">
         <v>442.56</v>
       </c>
+      <c r="I27" s="5">
+        <f t="shared" si="7"/>
+        <v>8.9499999999999886</v>
+      </c>
       <c r="J27">
-        <f t="shared" si="1"/>
-        <v>17.899999999999977</v>
+        <f>I27-I17</f>
+        <v>17</v>
+      </c>
+      <c r="M27">
+        <v>0</v>
+      </c>
+      <c r="N27">
+        <v>-1</v>
+      </c>
+      <c r="O27">
+        <v>0</v>
+      </c>
+      <c r="P27">
+        <v>-6.9458000000000002</v>
+      </c>
+      <c r="Q27">
+        <v>230.65</v>
+      </c>
+      <c r="R27">
+        <v>159.83000000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="M28">
+        <v>0</v>
+      </c>
+      <c r="N28">
+        <v>-1.5</v>
+      </c>
+      <c r="O28">
+        <v>0</v>
+      </c>
+      <c r="P28">
+        <v>-6.8986999999999998</v>
+      </c>
+      <c r="Q28">
+        <v>230.87</v>
+      </c>
+      <c r="R28">
+        <v>159.79</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="M29">
+        <v>0</v>
+      </c>
+      <c r="N29">
+        <v>-2</v>
+      </c>
+      <c r="O29">
+        <v>0</v>
+      </c>
+      <c r="P29">
+        <v>-6.8517000000000001</v>
+      </c>
+      <c r="Q29">
+        <v>231.02</v>
+      </c>
+      <c r="R29">
+        <v>159.78</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="M30">
+        <v>0</v>
+      </c>
+      <c r="N30">
+        <v>-2.5</v>
+      </c>
+      <c r="O30">
+        <v>0</v>
+      </c>
+      <c r="P30">
+        <v>-6.8048000000000002</v>
+      </c>
+      <c r="Q30">
+        <v>231.08</v>
+      </c>
+      <c r="R30">
+        <v>159.82</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <sortState ref="M20:R30">
+    <sortCondition descending="1" ref="N20"/>
+  </sortState>
+  <mergeCells count="10">
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="I15:J15"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="G1:H1"/>

</xml_diff>